<commit_message>
Began implementing vertical sprite changes
</commit_message>
<xml_diff>
--- a/Docs/Other/scratchpad.xlsx
+++ b/Docs/Other/scratchpad.xlsx
@@ -1,28 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\JCAP\Docs\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unkno\Desktop\JCAP\Docs\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC72D156-A185-4A42-88B7-244E00EF092D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sandbox" sheetId="1" r:id="rId1"/>
-    <sheet name="LONG-to-LONG (Bad) - Table 1-1" sheetId="2" r:id="rId2"/>
-    <sheet name="LONG-to-LONG (Good) - Table 1-1" sheetId="3" r:id="rId3"/>
-    <sheet name="Buffer-to-buffer - Table 1-1" sheetId="4" r:id="rId4"/>
+    <sheet name="Vertical Sprite Mgmt" sheetId="5" r:id="rId2"/>
+    <sheet name="LONG-to-LONG (Bad) - Table 1-1" sheetId="2" r:id="rId3"/>
+    <sheet name="LONG-to-LONG (Good) - Table 1-1" sheetId="3" r:id="rId4"/>
+    <sheet name="Buffer-to-buffer - Table 1-1" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="139">
   <si>
     <t>PASM Line</t>
   </si>
@@ -355,13 +364,97 @@
   </si>
   <si>
     <t>jmp</t>
+  </si>
+  <si>
+    <t>spyoff:</t>
+  </si>
+  <si>
+    <t>spysz = tall  ? 16 : 8</t>
+  </si>
+  <si>
+    <t>spyoff = mir ? spysz - (cursl - spypos) : cursl - spypos</t>
+  </si>
+  <si>
+    <t>spysz</t>
+  </si>
+  <si>
+    <t>spypos</t>
+  </si>
+  <si>
+    <t>spyoff</t>
+  </si>
+  <si>
+    <t>mirrored</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>cursl - spypos &lt;= spysz ?</t>
+  </si>
+  <si>
+    <t>NO: Skip sprite</t>
+  </si>
+  <si>
+    <t>SP 1 L 0</t>
+  </si>
+  <si>
+    <t>SP 1 L 1</t>
+  </si>
+  <si>
+    <t>SP 1 L 2</t>
+  </si>
+  <si>
+    <t>SP 1 L 3</t>
+  </si>
+  <si>
+    <t>SP 1 L 4</t>
+  </si>
+  <si>
+    <t>SP 1 L 5</t>
+  </si>
+  <si>
+    <t>SP 1 L 6</t>
+  </si>
+  <si>
+    <t>SP 1 L 7</t>
+  </si>
+  <si>
+    <t>SP 2 L 0</t>
+  </si>
+  <si>
+    <t>SP 2 L 1</t>
+  </si>
+  <si>
+    <t>SP 2 L 2</t>
+  </si>
+  <si>
+    <t>SP 2 L 3</t>
+  </si>
+  <si>
+    <t>SP 2 L 4</t>
+  </si>
+  <si>
+    <t>SP 2 L 5</t>
+  </si>
+  <si>
+    <t>SP 2 L 6</t>
+  </si>
+  <si>
+    <t>SP 2 L 7</t>
+  </si>
+  <si>
+    <t>NORMAL:</t>
+  </si>
+  <si>
+    <t>MIRRORED:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -414,8 +507,24 @@
       <color indexed="28"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -518,8 +627,50 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="56">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1264,11 +1415,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1443,6 +1699,35 @@
     <xf numFmtId="49" fontId="0" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1545,7 +1830,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Shape 2"/>
+        <xdr:cNvPr id="2" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2655,23 +2946,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV60"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.85" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.85" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="256" width="8.85546875" style="1" customWidth="1"/>
+    <col min="7" max="256" width="8.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2718,7 +3011,7 @@
       <c r="AH1" s="6"/>
       <c r="AI1" s="6"/>
     </row>
-    <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>162</v>
       </c>
@@ -2769,7 +3062,7 @@
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
     </row>
-    <row r="3" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>163</v>
       </c>
@@ -2818,7 +3111,7 @@
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>164</v>
       </c>
@@ -2867,7 +3160,7 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
     </row>
-    <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>165</v>
       </c>
@@ -2920,7 +3213,7 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
     </row>
-    <row r="6" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>166</v>
       </c>
@@ -2973,7 +3266,7 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="6"/>
     </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>167</v>
       </c>
@@ -3026,7 +3319,7 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="6"/>
     </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>168</v>
       </c>
@@ -3075,7 +3368,7 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="6"/>
     </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>169</v>
       </c>
@@ -3122,7 +3415,7 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>170</v>
       </c>
@@ -3169,7 +3462,7 @@
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" s="31"/>
       <c r="C11" s="24"/>
@@ -3208,7 +3501,7 @@
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
     </row>
-    <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -3253,7 +3546,7 @@
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
     </row>
-    <row r="13" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>26</v>
       </c>
@@ -3302,7 +3595,7 @@
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
         <v>26</v>
       </c>
@@ -3353,7 +3646,7 @@
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
     </row>
-    <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>26</v>
       </c>
@@ -3404,7 +3697,7 @@
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
     </row>
-    <row r="16" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>26</v>
       </c>
@@ -3451,7 +3744,7 @@
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>26</v>
       </c>
@@ -3498,7 +3791,7 @@
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
         <v>26</v>
       </c>
@@ -3545,7 +3838,7 @@
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>26</v>
       </c>
@@ -3592,7 +3885,7 @@
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="24"/>
@@ -3633,7 +3926,7 @@
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -3670,7 +3963,7 @@
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -3707,7 +4000,7 @@
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
     </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -3744,7 +4037,7 @@
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -3781,7 +4074,7 @@
       <c r="AH24" s="6"/>
       <c r="AI24" s="6"/>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -3818,7 +4111,7 @@
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="38" t="s">
@@ -3897,7 +4190,7 @@
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="38" t="s">
@@ -3946,7 +4239,7 @@
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="38" t="s">
@@ -4025,7 +4318,7 @@
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -4062,7 +4355,7 @@
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -4103,7 +4396,7 @@
       <c r="AH30" s="6"/>
       <c r="AI30" s="6"/>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="47"/>
@@ -4152,7 +4445,7 @@
       <c r="AH31" s="6"/>
       <c r="AI31" s="6"/>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="47"/>
@@ -4199,7 +4492,7 @@
       <c r="AH32" s="6"/>
       <c r="AI32" s="6"/>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="47"/>
@@ -4246,7 +4539,7 @@
       <c r="AH33" s="6"/>
       <c r="AI33" s="6"/>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="47"/>
@@ -4293,7 +4586,7 @@
       <c r="AH34" s="6"/>
       <c r="AI34" s="6"/>
     </row>
-    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="47"/>
@@ -4340,7 +4633,7 @@
       <c r="AH35" s="6"/>
       <c r="AI35" s="6"/>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="47"/>
@@ -4387,7 +4680,7 @@
       <c r="AH36" s="6"/>
       <c r="AI36" s="6"/>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="47"/>
@@ -4434,7 +4727,7 @@
       <c r="AH37" s="6"/>
       <c r="AI37" s="6"/>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="47"/>
@@ -4481,7 +4774,7 @@
       <c r="AH38" s="6"/>
       <c r="AI38" s="6"/>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="47"/>
@@ -4528,7 +4821,7 @@
       <c r="AH39" s="6"/>
       <c r="AI39" s="6"/>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -4565,7 +4858,7 @@
       <c r="AH40" s="6"/>
       <c r="AI40" s="6"/>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -4602,7 +4895,7 @@
       <c r="AH41" s="6"/>
       <c r="AI41" s="6"/>
     </row>
-    <row r="42" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -4639,7 +4932,7 @@
       <c r="AH42" s="5"/>
       <c r="AI42" s="5"/>
     </row>
-    <row r="43" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="56"/>
@@ -4684,7 +4977,7 @@
       <c r="AH43" s="101"/>
       <c r="AI43" s="102"/>
     </row>
-    <row r="44" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="56"/>
@@ -4737,7 +5030,7 @@
       <c r="AH44" s="98"/>
       <c r="AI44" s="99"/>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="38" t="s">
@@ -4840,7 +5133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="33" t="s">
@@ -4943,7 +5236,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -4980,7 +5273,7 @@
       <c r="AH47" s="6"/>
       <c r="AI47" s="6"/>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -5021,7 +5314,7 @@
       <c r="AH48" s="6"/>
       <c r="AI48" s="6"/>
     </row>
-    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -5062,7 +5355,7 @@
       <c r="AH49" s="6"/>
       <c r="AI49" s="6"/>
     </row>
-    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -5104,7 +5397,7 @@
       <c r="AH50" s="6"/>
       <c r="AI50" s="6"/>
     </row>
-    <row r="51" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -5141,7 +5434,7 @@
       <c r="AH51" s="6"/>
       <c r="AI51" s="6"/>
     </row>
-    <row r="52" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -5182,7 +5475,7 @@
       <c r="AH52" s="6"/>
       <c r="AI52" s="6"/>
     </row>
-    <row r="53" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -5227,7 +5520,7 @@
       <c r="AH53" s="6"/>
       <c r="AI53" s="6"/>
     </row>
-    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -5296,7 +5589,7 @@
       <c r="AH54" s="6"/>
       <c r="AI54" s="6"/>
     </row>
-    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -5365,7 +5658,7 @@
       <c r="AH55" s="6"/>
       <c r="AI55" s="6"/>
     </row>
-    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -5402,7 +5695,7 @@
       <c r="AH56" s="6"/>
       <c r="AI56" s="6"/>
     </row>
-    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -5439,7 +5732,7 @@
       <c r="AH57" s="6"/>
       <c r="AI57" s="6"/>
     </row>
-    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -5478,7 +5771,7 @@
       <c r="AH58" s="6"/>
       <c r="AI58" s="6"/>
     </row>
-    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -5521,7 +5814,7 @@
       <c r="AH59" s="6"/>
       <c r="AI59" s="6"/>
     </row>
-    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -5595,7 +5888,379 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91793D44-BCD1-44CE-9C40-D1F7D97CC6C2}">
+  <dimension ref="A1:J39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" style="108" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" style="109" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="115" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="110">
+        <v>0</v>
+      </c>
+      <c r="D1" s="106">
+        <v>1</v>
+      </c>
+      <c r="E1" s="107" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="114" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="111">
+        <v>2</v>
+      </c>
+      <c r="D2" s="108">
+        <v>2</v>
+      </c>
+      <c r="E2" s="119" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="120" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="120" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" s="120" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="111">
+        <v>16</v>
+      </c>
+      <c r="D3" s="108">
+        <v>3</v>
+      </c>
+      <c r="E3" s="119" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="115" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="121" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="117" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="112" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="108">
+        <v>4</v>
+      </c>
+      <c r="E4" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="114" t="s">
+        <v>122</v>
+      </c>
+      <c r="J4" s="122" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="124">
+        <f>IF(B4,B3-(B1-B2),B1-B2)</f>
+        <v>-2</v>
+      </c>
+      <c r="D5" s="108">
+        <v>5</v>
+      </c>
+      <c r="G5" s="114" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="122" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="113" t="str">
+        <f>IF(IF((B1-B2)&lt;0, 4294967295, B1-B2)&lt;B3, "YES", "NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="D6" s="108">
+        <v>6</v>
+      </c>
+      <c r="G6" s="114" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="122" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D7" s="108">
+        <v>7</v>
+      </c>
+      <c r="G7" s="114" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="122" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D8" s="108">
+        <v>8</v>
+      </c>
+      <c r="G8" s="114" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="122" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D9" s="108">
+        <v>9</v>
+      </c>
+      <c r="G9" s="114" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" s="122" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="108">
+        <v>10</v>
+      </c>
+      <c r="G10" s="117" t="s">
+        <v>128</v>
+      </c>
+      <c r="J10" s="123" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D11" s="108">
+        <v>11</v>
+      </c>
+      <c r="G11" s="121" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11" s="115" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D12" s="108">
+        <v>12</v>
+      </c>
+      <c r="G12" s="122" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" s="114" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D13" s="108">
+        <v>13</v>
+      </c>
+      <c r="G13" s="122" t="s">
+        <v>131</v>
+      </c>
+      <c r="J13" s="114" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D14" s="108">
+        <v>14</v>
+      </c>
+      <c r="G14" s="122" t="s">
+        <v>132</v>
+      </c>
+      <c r="J14" s="114" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D15" s="108">
+        <v>15</v>
+      </c>
+      <c r="G15" s="122" t="s">
+        <v>133</v>
+      </c>
+      <c r="J15" s="114" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D16" s="108">
+        <v>16</v>
+      </c>
+      <c r="G16" s="122" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="114" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17" s="108">
+        <v>17</v>
+      </c>
+      <c r="G17" s="122" t="s">
+        <v>135</v>
+      </c>
+      <c r="J17" s="114" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="108">
+        <v>18</v>
+      </c>
+      <c r="G18" s="123" t="s">
+        <v>136</v>
+      </c>
+      <c r="J18" s="117" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D19" s="108">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="108">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D21" s="108">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D22" s="108">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="108">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="108">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D25" s="108">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="108">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D27" s="108">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D28" s="108">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D29" s="108">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D30" s="108">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D31" s="108">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D32" s="108">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="108">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="108">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="108">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" s="108">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" s="108">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="108">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" s="108">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5603,12 +6268,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.85" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.85" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="256" width="8.85546875" style="64" customWidth="1"/>
+    <col min="1" max="256" width="8.88671875" style="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="65" t="s">
         <v>66</v>
@@ -5626,7 +6291,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="67" t="s">
         <v>68</v>
@@ -5648,7 +6313,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="105" t="s">
         <v>70</v>
       </c>
@@ -5672,7 +6337,7 @@
       <c r="K3" s="71"/>
       <c r="L3" s="71"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="104"/>
       <c r="B4" s="69" t="s">
         <v>71</v>
@@ -5694,7 +6359,7 @@
       <c r="K4" s="71"/>
       <c r="L4" s="71"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="104"/>
       <c r="B5" s="78"/>
       <c r="C5" s="73">
@@ -5713,7 +6378,7 @@
       <c r="K5" s="71"/>
       <c r="L5" s="71"/>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="104"/>
       <c r="B6" s="78"/>
       <c r="C6" s="73">
@@ -5734,7 +6399,7 @@
       <c r="K6" s="71"/>
       <c r="L6" s="71"/>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104"/>
       <c r="B7" s="78"/>
       <c r="C7" s="73">
@@ -5755,7 +6420,7 @@
       <c r="K7" s="71"/>
       <c r="L7" s="71"/>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="104"/>
       <c r="B8" s="69" t="s">
         <v>71</v>
@@ -5782,7 +6447,7 @@
       <c r="K8" s="71"/>
       <c r="L8" s="71"/>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="104"/>
       <c r="B9" s="78"/>
       <c r="C9" s="73">
@@ -5806,7 +6471,7 @@
       <c r="K9" s="71"/>
       <c r="L9" s="71"/>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="104"/>
       <c r="B10" s="78"/>
       <c r="C10" s="73">
@@ -5830,7 +6495,7 @@
       <c r="K10" s="71"/>
       <c r="L10" s="71"/>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="104"/>
       <c r="B11" s="78"/>
       <c r="C11" s="73">
@@ -5854,7 +6519,7 @@
       <c r="K11" s="71"/>
       <c r="L11" s="71"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="104"/>
       <c r="B12" s="69" t="s">
         <v>81</v>
@@ -5878,7 +6543,7 @@
       <c r="K12" s="71"/>
       <c r="L12" s="71"/>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="104"/>
       <c r="B13" s="78"/>
       <c r="C13" s="73">
@@ -5902,7 +6567,7 @@
       <c r="K13" s="71"/>
       <c r="L13" s="71"/>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="104"/>
       <c r="B14" s="78"/>
       <c r="C14" s="73">
@@ -5924,7 +6589,7 @@
       <c r="K14" s="71"/>
       <c r="L14" s="71"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="104"/>
       <c r="B15" s="78"/>
       <c r="C15" s="73">
@@ -5948,7 +6613,7 @@
       <c r="K15" s="71"/>
       <c r="L15" s="71"/>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="104"/>
       <c r="B16" s="69" t="s">
         <v>85</v>
@@ -5972,7 +6637,7 @@
       <c r="K16" s="71"/>
       <c r="L16" s="71"/>
     </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="104"/>
       <c r="B17" s="78"/>
       <c r="C17" s="73">
@@ -5994,7 +6659,7 @@
       <c r="K17" s="71"/>
       <c r="L17" s="71"/>
     </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="104"/>
       <c r="B18" s="78"/>
       <c r="C18" s="73">
@@ -6016,7 +6681,7 @@
       <c r="K18" s="71"/>
       <c r="L18" s="71"/>
     </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="104"/>
       <c r="B19" s="78"/>
       <c r="C19" s="73">
@@ -6040,7 +6705,7 @@
       <c r="K19" s="71"/>
       <c r="L19" s="71"/>
     </row>
-    <row r="20" spans="1:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="104"/>
       <c r="B20" s="69" t="s">
         <v>88</v>
@@ -6063,7 +6728,7 @@
       <c r="K20" s="71"/>
       <c r="L20" s="71"/>
     </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="104"/>
       <c r="B21" s="78"/>
       <c r="C21" s="70" t="s">
@@ -6083,7 +6748,7 @@
       <c r="K21" s="71"/>
       <c r="L21" s="71"/>
     </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="104"/>
       <c r="B22" s="69" t="s">
         <v>90</v>
@@ -6107,7 +6772,7 @@
       <c r="K22" s="71"/>
       <c r="L22" s="71"/>
     </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="104"/>
       <c r="B23" s="78"/>
       <c r="C23" s="73">
@@ -6131,7 +6796,7 @@
       <c r="K23" s="71"/>
       <c r="L23" s="71"/>
     </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="104"/>
       <c r="B24" s="78"/>
       <c r="C24" s="73">
@@ -6153,7 +6818,7 @@
       <c r="K24" s="71"/>
       <c r="L24" s="71"/>
     </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="104"/>
       <c r="B25" s="78"/>
       <c r="C25" s="73">
@@ -6177,7 +6842,7 @@
       <c r="K25" s="71"/>
       <c r="L25" s="71"/>
     </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="104"/>
       <c r="B26" s="78"/>
       <c r="C26" s="73">
@@ -6199,7 +6864,7 @@
       <c r="K26" s="71"/>
       <c r="L26" s="71"/>
     </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="104"/>
       <c r="B27" s="78"/>
       <c r="C27" s="73">
@@ -6219,7 +6884,7 @@
       <c r="K27" s="71"/>
       <c r="L27" s="71"/>
     </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="104"/>
       <c r="B28" s="78"/>
       <c r="C28" s="73">
@@ -6239,7 +6904,7 @@
       <c r="K28" s="71"/>
       <c r="L28" s="71"/>
     </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="104"/>
       <c r="B29" s="78"/>
       <c r="C29" s="73">
@@ -6263,7 +6928,7 @@
       <c r="K29" s="71"/>
       <c r="L29" s="71"/>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="104"/>
       <c r="B30" s="69" t="s">
         <v>71</v>
@@ -6287,7 +6952,7 @@
       <c r="K30" s="71"/>
       <c r="L30" s="71"/>
     </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="103" t="s">
         <v>97</v>
       </c>
@@ -6313,7 +6978,7 @@
       <c r="K31" s="87"/>
       <c r="L31" s="87"/>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="104"/>
       <c r="B32" s="69" t="s">
         <v>100</v>
@@ -6339,7 +7004,7 @@
       <c r="K32" s="87"/>
       <c r="L32" s="87"/>
     </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="104"/>
       <c r="B33" s="69" t="s">
         <v>96</v>
@@ -6363,7 +7028,7 @@
       <c r="K33" s="87"/>
       <c r="L33" s="87"/>
     </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="104"/>
       <c r="B34" s="69" t="s">
         <v>71</v>
@@ -6389,7 +7054,7 @@
       <c r="K34" s="87"/>
       <c r="L34" s="87"/>
     </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="104"/>
       <c r="B35" s="69" t="s">
         <v>71</v>
@@ -6410,7 +7075,7 @@
       <c r="K35" s="87"/>
       <c r="L35" s="87"/>
     </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="104"/>
       <c r="B36" s="78"/>
       <c r="C36" s="73">
@@ -6427,7 +7092,7 @@
       <c r="K36" s="87"/>
       <c r="L36" s="87"/>
     </row>
-    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="104"/>
       <c r="B37" s="78"/>
       <c r="C37" s="73">
@@ -6444,7 +7109,7 @@
       <c r="K37" s="87"/>
       <c r="L37" s="87"/>
     </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="104"/>
       <c r="B38" s="78"/>
       <c r="C38" s="73">
@@ -6463,7 +7128,7 @@
       <c r="K38" s="87"/>
       <c r="L38" s="87"/>
     </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="104"/>
       <c r="B39" s="69" t="s">
         <v>71</v>
@@ -6484,7 +7149,7 @@
       <c r="K39" s="87"/>
       <c r="L39" s="87"/>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="104"/>
       <c r="B40" s="78"/>
       <c r="C40" s="73">
@@ -6503,7 +7168,7 @@
       <c r="K40" s="87"/>
       <c r="L40" s="87"/>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="104"/>
       <c r="B41" s="78"/>
       <c r="C41" s="73">
@@ -6522,7 +7187,7 @@
       <c r="K41" s="87"/>
       <c r="L41" s="87"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="104"/>
       <c r="B42" s="78"/>
       <c r="C42" s="73">
@@ -6541,7 +7206,7 @@
       <c r="K42" s="87"/>
       <c r="L42" s="87"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="104"/>
       <c r="B43" s="69" t="s">
         <v>81</v>
@@ -6562,7 +7227,7 @@
       <c r="K43" s="87"/>
       <c r="L43" s="87"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="104"/>
       <c r="B44" s="78"/>
       <c r="C44" s="73">
@@ -6581,7 +7246,7 @@
       <c r="K44" s="87"/>
       <c r="L44" s="87"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="104"/>
       <c r="B45" s="78"/>
       <c r="C45" s="73">
@@ -6600,7 +7265,7 @@
       <c r="K45" s="87"/>
       <c r="L45" s="87"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="104"/>
       <c r="B46" s="78"/>
       <c r="C46" s="73">
@@ -6619,7 +7284,7 @@
       <c r="K46" s="87"/>
       <c r="L46" s="87"/>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="104"/>
       <c r="B47" s="69" t="s">
         <v>85</v>
@@ -6654,8 +7319,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6663,12 +7328,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.85" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.85" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="256" width="8.85546875" style="92" customWidth="1"/>
+    <col min="1" max="256" width="8.88671875" style="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="65" t="s">
         <v>66</v>
@@ -6685,7 +7350,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="67" t="s">
         <v>68</v>
@@ -6706,7 +7371,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="105" t="s">
         <v>70</v>
       </c>
@@ -6729,7 +7394,7 @@
       <c r="J3" s="71"/>
       <c r="K3" s="71"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="104"/>
       <c r="B4" s="69" t="s">
         <v>71</v>
@@ -6750,7 +7415,7 @@
       <c r="J4" s="71"/>
       <c r="K4" s="71"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="104"/>
       <c r="B5" s="78"/>
       <c r="C5" s="73">
@@ -6768,7 +7433,7 @@
       <c r="J5" s="71"/>
       <c r="K5" s="71"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="104"/>
       <c r="B6" s="78"/>
       <c r="C6" s="73">
@@ -6788,7 +7453,7 @@
       <c r="J6" s="71"/>
       <c r="K6" s="71"/>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104"/>
       <c r="B7" s="78"/>
       <c r="C7" s="73">
@@ -6808,7 +7473,7 @@
       <c r="J7" s="71"/>
       <c r="K7" s="71"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="104"/>
       <c r="B8" s="69" t="s">
         <v>71</v>
@@ -6834,7 +7499,7 @@
       <c r="J8" s="71"/>
       <c r="K8" s="71"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="104"/>
       <c r="B9" s="78"/>
       <c r="C9" s="73">
@@ -6857,7 +7522,7 @@
       <c r="J9" s="71"/>
       <c r="K9" s="71"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="104"/>
       <c r="B10" s="78"/>
       <c r="C10" s="73">
@@ -6880,7 +7545,7 @@
       <c r="J10" s="71"/>
       <c r="K10" s="71"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="104"/>
       <c r="B11" s="78"/>
       <c r="C11" s="73">
@@ -6903,7 +7568,7 @@
       <c r="J11" s="71"/>
       <c r="K11" s="71"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="104"/>
       <c r="B12" s="69" t="s">
         <v>81</v>
@@ -6926,7 +7591,7 @@
       <c r="J12" s="71"/>
       <c r="K12" s="71"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="104"/>
       <c r="B13" s="78"/>
       <c r="C13" s="73">
@@ -6949,7 +7614,7 @@
       <c r="J13" s="71"/>
       <c r="K13" s="71"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="104"/>
       <c r="B14" s="78"/>
       <c r="C14" s="73">
@@ -6970,7 +7635,7 @@
       <c r="J14" s="71"/>
       <c r="K14" s="71"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="104"/>
       <c r="B15" s="78"/>
       <c r="C15" s="73">
@@ -6993,7 +7658,7 @@
       <c r="J15" s="71"/>
       <c r="K15" s="71"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="104"/>
       <c r="B16" s="69" t="s">
         <v>85</v>
@@ -7016,7 +7681,7 @@
       <c r="J16" s="71"/>
       <c r="K16" s="71"/>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="104"/>
       <c r="B17" s="78"/>
       <c r="C17" s="73">
@@ -7037,7 +7702,7 @@
       <c r="J17" s="71"/>
       <c r="K17" s="71"/>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="104"/>
       <c r="B18" s="78"/>
       <c r="C18" s="73">
@@ -7058,7 +7723,7 @@
       <c r="J18" s="71"/>
       <c r="K18" s="71"/>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="104"/>
       <c r="B19" s="78"/>
       <c r="C19" s="73">
@@ -7081,7 +7746,7 @@
       <c r="J19" s="71"/>
       <c r="K19" s="71"/>
     </row>
-    <row r="20" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="104"/>
       <c r="B20" s="69" t="s">
         <v>88</v>
@@ -7103,7 +7768,7 @@
       <c r="J20" s="71"/>
       <c r="K20" s="71"/>
     </row>
-    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="104"/>
       <c r="B21" s="78"/>
       <c r="C21" s="70" t="s">
@@ -7122,7 +7787,7 @@
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
     </row>
-    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="104"/>
       <c r="B22" s="69" t="s">
         <v>90</v>
@@ -7145,7 +7810,7 @@
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
     </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="104"/>
       <c r="B23" s="78"/>
       <c r="C23" s="73">
@@ -7168,7 +7833,7 @@
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="104"/>
       <c r="B24" s="78"/>
       <c r="C24" s="73">
@@ -7189,7 +7854,7 @@
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
     </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="104"/>
       <c r="B25" s="78"/>
       <c r="C25" s="73">
@@ -7212,7 +7877,7 @@
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
     </row>
-    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="104"/>
       <c r="B26" s="78"/>
       <c r="C26" s="73">
@@ -7233,7 +7898,7 @@
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
     </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="104"/>
       <c r="B27" s="78"/>
       <c r="C27" s="73">
@@ -7252,7 +7917,7 @@
       <c r="J27" s="71"/>
       <c r="K27" s="71"/>
     </row>
-    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="104"/>
       <c r="B28" s="78"/>
       <c r="C28" s="73">
@@ -7271,7 +7936,7 @@
       <c r="J28" s="71"/>
       <c r="K28" s="71"/>
     </row>
-    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="104"/>
       <c r="B29" s="78"/>
       <c r="C29" s="73">
@@ -7292,7 +7957,7 @@
       <c r="J29" s="71"/>
       <c r="K29" s="71"/>
     </row>
-    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="104"/>
       <c r="B30" s="69" t="s">
         <v>71</v>
@@ -7315,7 +7980,7 @@
       <c r="J30" s="71"/>
       <c r="K30" s="71"/>
     </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="103" t="s">
         <v>97</v>
       </c>
@@ -7340,7 +8005,7 @@
       <c r="J31" s="87"/>
       <c r="K31" s="87"/>
     </row>
-    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="104"/>
       <c r="B32" s="69" t="s">
         <v>100</v>
@@ -7363,7 +8028,7 @@
       <c r="J32" s="87"/>
       <c r="K32" s="87"/>
     </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="104"/>
       <c r="B33" s="69" t="s">
         <v>96</v>
@@ -7384,7 +8049,7 @@
       <c r="J33" s="87"/>
       <c r="K33" s="87"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="104"/>
       <c r="B34" s="69" t="s">
         <v>71</v>
@@ -7407,7 +8072,7 @@
       <c r="J34" s="87"/>
       <c r="K34" s="87"/>
     </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="104"/>
       <c r="B35" s="69" t="s">
         <v>105</v>
@@ -7430,7 +8095,7 @@
       <c r="J35" s="87"/>
       <c r="K35" s="87"/>
     </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="104"/>
       <c r="B36" s="69" t="s">
         <v>105</v>
@@ -7448,7 +8113,7 @@
       <c r="J36" s="87"/>
       <c r="K36" s="87"/>
     </row>
-    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="104"/>
       <c r="B37" s="69" t="s">
         <v>105</v>
@@ -7466,7 +8131,7 @@
       <c r="J37" s="87"/>
       <c r="K37" s="87"/>
     </row>
-    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="104"/>
       <c r="B38" s="69" t="s">
         <v>71</v>
@@ -7484,7 +8149,7 @@
       <c r="J38" s="87"/>
       <c r="K38" s="87"/>
     </row>
-    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="104"/>
       <c r="B39" s="78"/>
       <c r="C39" s="73">
@@ -7500,7 +8165,7 @@
       <c r="J39" s="87"/>
       <c r="K39" s="87"/>
     </row>
-    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="104"/>
       <c r="B40" s="78"/>
       <c r="C40" s="73">
@@ -7516,7 +8181,7 @@
       <c r="J40" s="87"/>
       <c r="K40" s="87"/>
     </row>
-    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="104"/>
       <c r="B41" s="78"/>
       <c r="C41" s="73">
@@ -7534,7 +8199,7 @@
       <c r="J41" s="87"/>
       <c r="K41" s="87"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="104"/>
       <c r="B42" s="69" t="s">
         <v>71</v>
@@ -7554,7 +8219,7 @@
       <c r="J42" s="87"/>
       <c r="K42" s="87"/>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="104"/>
       <c r="B43" s="78"/>
       <c r="C43" s="73">
@@ -7572,7 +8237,7 @@
       <c r="J43" s="87"/>
       <c r="K43" s="87"/>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="104"/>
       <c r="B44" s="78"/>
       <c r="C44" s="73">
@@ -7590,7 +8255,7 @@
       <c r="J44" s="87"/>
       <c r="K44" s="87"/>
     </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="104"/>
       <c r="B45" s="78"/>
       <c r="C45" s="73">
@@ -7608,7 +8273,7 @@
       <c r="J45" s="87"/>
       <c r="K45" s="87"/>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="104"/>
       <c r="B46" s="69" t="s">
         <v>81</v>
@@ -7628,7 +8293,7 @@
       <c r="J46" s="87"/>
       <c r="K46" s="87"/>
     </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="104"/>
       <c r="B47" s="78"/>
       <c r="C47" s="73">
@@ -7646,7 +8311,7 @@
       <c r="J47" s="87"/>
       <c r="K47" s="87"/>
     </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="104"/>
       <c r="B48" s="78"/>
       <c r="C48" s="73">
@@ -7664,7 +8329,7 @@
       <c r="J48" s="87"/>
       <c r="K48" s="87"/>
     </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="104"/>
       <c r="B49" s="78"/>
       <c r="C49" s="73">
@@ -7682,7 +8347,7 @@
       <c r="J49" s="87"/>
       <c r="K49" s="87"/>
     </row>
-    <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="104"/>
       <c r="B50" s="69" t="s">
         <v>85</v>
@@ -7715,23 +8380,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IV58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.85" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.85" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="256" width="8.85546875" style="94" customWidth="1"/>
+    <col min="1" max="256" width="8.88671875" style="94" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="65" t="s">
         <v>66</v>
@@ -7748,7 +8413,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="67" t="s">
         <v>68</v>
@@ -7769,7 +8434,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="105" t="s">
         <v>106</v>
       </c>
@@ -7792,7 +8457,7 @@
       <c r="J3" s="71"/>
       <c r="K3" s="71"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="104"/>
       <c r="B4" s="69" t="s">
         <v>71</v>
@@ -7813,7 +8478,7 @@
       <c r="J4" s="71"/>
       <c r="K4" s="71"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="104"/>
       <c r="B5" s="78"/>
       <c r="C5" s="73">
@@ -7831,7 +8496,7 @@
       <c r="J5" s="71"/>
       <c r="K5" s="71"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="104"/>
       <c r="B6" s="78"/>
       <c r="C6" s="73">
@@ -7851,7 +8516,7 @@
       <c r="J6" s="71"/>
       <c r="K6" s="71"/>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104"/>
       <c r="B7" s="78"/>
       <c r="C7" s="73">
@@ -7871,7 +8536,7 @@
       <c r="J7" s="71"/>
       <c r="K7" s="71"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="104"/>
       <c r="B8" s="69" t="s">
         <v>71</v>
@@ -7897,7 +8562,7 @@
       <c r="J8" s="71"/>
       <c r="K8" s="71"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="104"/>
       <c r="B9" s="78"/>
       <c r="C9" s="73">
@@ -7920,7 +8585,7 @@
       <c r="J9" s="71"/>
       <c r="K9" s="71"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="104"/>
       <c r="B10" s="78"/>
       <c r="C10" s="73">
@@ -7943,7 +8608,7 @@
       <c r="J10" s="71"/>
       <c r="K10" s="71"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="104"/>
       <c r="B11" s="78"/>
       <c r="C11" s="73">
@@ -7966,7 +8631,7 @@
       <c r="J11" s="71"/>
       <c r="K11" s="71"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="104"/>
       <c r="B12" s="69" t="s">
         <v>81</v>
@@ -7989,7 +8654,7 @@
       <c r="J12" s="71"/>
       <c r="K12" s="71"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="104"/>
       <c r="B13" s="78"/>
       <c r="C13" s="73">
@@ -8012,7 +8677,7 @@
       <c r="J13" s="71"/>
       <c r="K13" s="71"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="104"/>
       <c r="B14" s="78"/>
       <c r="C14" s="73">
@@ -8033,7 +8698,7 @@
       <c r="J14" s="71"/>
       <c r="K14" s="71"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="104"/>
       <c r="B15" s="78"/>
       <c r="C15" s="73">
@@ -8056,7 +8721,7 @@
       <c r="J15" s="71"/>
       <c r="K15" s="71"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="104"/>
       <c r="B16" s="69" t="s">
         <v>85</v>
@@ -8079,7 +8744,7 @@
       <c r="J16" s="71"/>
       <c r="K16" s="71"/>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="104"/>
       <c r="B17" s="78"/>
       <c r="C17" s="73">
@@ -8100,7 +8765,7 @@
       <c r="J17" s="71"/>
       <c r="K17" s="71"/>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="104"/>
       <c r="B18" s="78"/>
       <c r="C18" s="73">
@@ -8121,7 +8786,7 @@
       <c r="J18" s="71"/>
       <c r="K18" s="71"/>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="104"/>
       <c r="B19" s="78"/>
       <c r="C19" s="73">
@@ -8144,7 +8809,7 @@
       <c r="J19" s="71"/>
       <c r="K19" s="71"/>
     </row>
-    <row r="20" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="104"/>
       <c r="B20" s="69" t="s">
         <v>88</v>
@@ -8166,7 +8831,7 @@
       <c r="J20" s="71"/>
       <c r="K20" s="71"/>
     </row>
-    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="104"/>
       <c r="B21" s="78"/>
       <c r="C21" s="70" t="s">
@@ -8185,7 +8850,7 @@
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
     </row>
-    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="104"/>
       <c r="B22" s="69" t="s">
         <v>90</v>
@@ -8208,7 +8873,7 @@
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
     </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="104"/>
       <c r="B23" s="78"/>
       <c r="C23" s="73">
@@ -8231,7 +8896,7 @@
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="104"/>
       <c r="B24" s="78"/>
       <c r="C24" s="73">
@@ -8252,7 +8917,7 @@
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
     </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="104"/>
       <c r="B25" s="78"/>
       <c r="C25" s="73">
@@ -8275,7 +8940,7 @@
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
     </row>
-    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="104"/>
       <c r="B26" s="78"/>
       <c r="C26" s="73">
@@ -8296,7 +8961,7 @@
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
     </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="104"/>
       <c r="B27" s="78"/>
       <c r="C27" s="73">
@@ -8315,7 +8980,7 @@
       <c r="J27" s="71"/>
       <c r="K27" s="71"/>
     </row>
-    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="104"/>
       <c r="B28" s="78"/>
       <c r="C28" s="73">
@@ -8334,7 +8999,7 @@
       <c r="J28" s="71"/>
       <c r="K28" s="71"/>
     </row>
-    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="104"/>
       <c r="B29" s="78"/>
       <c r="C29" s="73">
@@ -8355,7 +9020,7 @@
       <c r="J29" s="71"/>
       <c r="K29" s="71"/>
     </row>
-    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="104"/>
       <c r="B30" s="69" t="s">
         <v>71</v>
@@ -8378,7 +9043,7 @@
       <c r="J30" s="71"/>
       <c r="K30" s="71"/>
     </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="103" t="s">
         <v>70</v>
       </c>
@@ -8403,7 +9068,7 @@
       <c r="J31" s="87"/>
       <c r="K31" s="87"/>
     </row>
-    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="104"/>
       <c r="B32" s="69" t="s">
         <v>107</v>
@@ -8426,7 +9091,7 @@
       <c r="J32" s="87"/>
       <c r="K32" s="87"/>
     </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="104"/>
       <c r="B33" s="69" t="s">
         <v>72</v>
@@ -8447,7 +9112,7 @@
       <c r="J33" s="87"/>
       <c r="K33" s="87"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="104"/>
       <c r="B34" s="78"/>
       <c r="C34" s="73">
@@ -8466,7 +9131,7 @@
       <c r="J34" s="87"/>
       <c r="K34" s="87"/>
     </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="104"/>
       <c r="B35" s="78"/>
       <c r="C35" s="73">
@@ -8489,7 +9154,7 @@
       <c r="J35" s="87"/>
       <c r="K35" s="87"/>
     </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="104"/>
       <c r="B36" s="78"/>
       <c r="C36" s="70" t="s">
@@ -8511,7 +9176,7 @@
       <c r="J36" s="87"/>
       <c r="K36" s="87"/>
     </row>
-    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="104"/>
       <c r="B37" s="78"/>
       <c r="C37" s="73">
@@ -8535,7 +9200,7 @@
       <c r="J37" s="87"/>
       <c r="K37" s="87"/>
     </row>
-    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="104"/>
       <c r="B38" s="78"/>
       <c r="C38" s="73">
@@ -8558,7 +9223,7 @@
       <c r="J38" s="87"/>
       <c r="K38" s="87"/>
     </row>
-    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="104"/>
       <c r="B39" s="78"/>
       <c r="C39" s="73">
@@ -8579,7 +9244,7 @@
       <c r="J39" s="87"/>
       <c r="K39" s="87"/>
     </row>
-    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="104"/>
       <c r="B40" s="69" t="s">
         <v>108</v>
@@ -8602,7 +9267,7 @@
       <c r="J40" s="87"/>
       <c r="K40" s="87"/>
     </row>
-    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="104"/>
       <c r="B41" s="69" t="s">
         <v>94</v>
@@ -8625,7 +9290,7 @@
       <c r="J41" s="87"/>
       <c r="K41" s="87"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="104"/>
       <c r="B42" s="69" t="s">
         <v>110</v>
@@ -8648,7 +9313,7 @@
       <c r="J42" s="87"/>
       <c r="K42" s="87"/>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="104"/>
       <c r="B43" s="69" t="s">
         <v>71</v>
@@ -8671,7 +9336,7 @@
       <c r="J43" s="87"/>
       <c r="K43" s="87"/>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="104"/>
       <c r="B44" s="69" t="s">
         <v>71</v>
@@ -8692,7 +9357,7 @@
       <c r="J44" s="87"/>
       <c r="K44" s="87"/>
     </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="104"/>
       <c r="B45" s="69" t="s">
         <v>100</v>
@@ -8715,7 +9380,7 @@
       <c r="J45" s="87"/>
       <c r="K45" s="87"/>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="104"/>
       <c r="B46" s="69" t="s">
         <v>110</v>
@@ -8735,7 +9400,7 @@
       <c r="J46" s="87"/>
       <c r="K46" s="87"/>
     </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="104"/>
       <c r="B47" s="69" t="s">
         <v>100</v>
@@ -8759,7 +9424,7 @@
       <c r="J47" s="87"/>
       <c r="K47" s="87"/>
     </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="104"/>
       <c r="B48" s="69" t="s">
         <v>96</v>
@@ -8782,7 +9447,7 @@
       <c r="J48" s="87"/>
       <c r="K48" s="87"/>
     </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="104"/>
       <c r="B49" s="69" t="s">
         <v>71</v>
@@ -8805,7 +9470,7 @@
       <c r="J49" s="87"/>
       <c r="K49" s="87"/>
     </row>
-    <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="104"/>
       <c r="B50" s="69" t="s">
         <v>71</v>
@@ -8828,7 +9493,7 @@
       <c r="J50" s="87"/>
       <c r="K50" s="87"/>
     </row>
-    <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="104"/>
       <c r="B51" s="78"/>
       <c r="C51" s="73">
@@ -8847,7 +9512,7 @@
       <c r="J51" s="87"/>
       <c r="K51" s="87"/>
     </row>
-    <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="104"/>
       <c r="B52" s="78"/>
       <c r="C52" s="73">
@@ -8868,7 +9533,7 @@
       <c r="J52" s="87"/>
       <c r="K52" s="87"/>
     </row>
-    <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="104"/>
       <c r="B53" s="78"/>
       <c r="C53" s="73">
@@ -8889,7 +9554,7 @@
       <c r="J53" s="87"/>
       <c r="K53" s="87"/>
     </row>
-    <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="104"/>
       <c r="B54" s="69" t="s">
         <v>71</v>
@@ -8914,7 +9579,7 @@
       <c r="J54" s="87"/>
       <c r="K54" s="87"/>
     </row>
-    <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="104"/>
       <c r="B55" s="78"/>
       <c r="C55" s="73">
@@ -8928,7 +9593,7 @@
       <c r="J55" s="87"/>
       <c r="K55" s="87"/>
     </row>
-    <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="104"/>
       <c r="B56" s="78"/>
       <c r="C56" s="73">
@@ -8946,7 +9611,7 @@
       <c r="J56" s="87"/>
       <c r="K56" s="87"/>
     </row>
-    <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="104"/>
       <c r="B57" s="78"/>
       <c r="C57" s="73">
@@ -8964,7 +9629,7 @@
       <c r="J57" s="87"/>
       <c r="K57" s="87"/>
     </row>
-    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="104"/>
       <c r="B58" s="78"/>
       <c r="C58" s="73">

</xml_diff>

<commit_message>
Successfully implemented vertical sprite sizing+mirroring!
</commit_message>
<xml_diff>
--- a/Docs/Other/scratchpad.xlsx
+++ b/Docs/Other/scratchpad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unkno\Desktop\JCAP\Docs\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC72D156-A185-4A42-88B7-244E00EF092D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CE2A1A-80A4-4B21-83FB-A0C9144FC658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,9 +372,6 @@
     <t>spysz = tall  ? 16 : 8</t>
   </si>
   <si>
-    <t>spyoff = mir ? spysz - (cursl - spypos) : cursl - spypos</t>
-  </si>
-  <si>
     <t>spysz</t>
   </si>
   <si>
@@ -448,6 +445,9 @@
   </si>
   <si>
     <t>MIRRORED:</t>
+  </si>
+  <si>
+    <t>spyoff = mir ? spysz - (cursl - spypos) - 1 : cursl - spypos</t>
   </si>
 </sst>
 </file>
@@ -5889,10 +5889,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91793D44-BCD1-44CE-9C40-D1F7D97CC6C2}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5900,15 +5900,15 @@
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5546875" style="108" customWidth="1"/>
-    <col min="5" max="5" width="43.44140625" style="109" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" style="109" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="115" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="110">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D1" s="106">
         <v>1</v>
@@ -5917,32 +5917,32 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="111">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="108">
         <v>2</v>
       </c>
       <c r="E2" s="119" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2" s="120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H2" s="120" t="s">
         <v>111</v>
       </c>
       <c r="J2" s="120" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="111">
         <v>16</v>
@@ -5951,269 +5951,493 @@
         <v>3</v>
       </c>
       <c r="E3" s="119" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="115" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="115" t="s">
-        <v>121</v>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>_xlfn.FLOOR.MATH(H3/8)</f>
+        <v>0</v>
       </c>
       <c r="J3" s="121" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+      <c r="K3">
+        <v>15</v>
+      </c>
+      <c r="L3">
+        <f>_xlfn.FLOOR.MATH(K3/8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="117" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="108">
         <v>4</v>
       </c>
-      <c r="E4" s="109" t="s">
-        <v>113</v>
+      <c r="E4" s="119" t="s">
+        <v>138</v>
       </c>
       <c r="G4" s="114" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I18" si="0">_xlfn.FLOOR.MATH(H4/8)</f>
+        <v>0</v>
       </c>
       <c r="J4" s="122" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L18" si="1">_xlfn.FLOOR.MATH(K4/8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="116" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="124">
-        <f>IF(B4,B3-(B1-B2),B1-B2)</f>
-        <v>-2</v>
+        <f>IF(B4,B3-(B1-B2)-1,B1-B2)</f>
+        <v>0</v>
       </c>
       <c r="D5" s="108">
         <v>5</v>
       </c>
       <c r="G5" s="114" t="s">
-        <v>123</v>
+        <v>122</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J5" s="122" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+      <c r="K5">
+        <v>13</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="118" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="113" t="str">
         <f>IF(IF((B1-B2)&lt;0, 4294967295, B1-B2)&lt;B3, "YES", "NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="D6" s="108">
         <v>6</v>
       </c>
       <c r="G6" s="114" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J6" s="122" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D7" s="108">
         <v>7</v>
       </c>
       <c r="G7" s="114" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J7" s="122" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D8" s="108">
         <v>8</v>
       </c>
       <c r="G8" s="114" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J8" s="122" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D9" s="108">
         <v>9</v>
       </c>
       <c r="G9" s="114" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J9" s="122" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="108">
         <v>10</v>
       </c>
       <c r="G10" s="117" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="123" t="s">
         <v>128</v>
       </c>
-      <c r="J10" s="123" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D11" s="108">
         <v>11</v>
       </c>
       <c r="G11" s="121" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J11" s="115" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D12" s="108">
         <v>12</v>
       </c>
       <c r="G12" s="122" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="H12">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J12" s="114" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D13" s="108">
         <v>13</v>
       </c>
       <c r="G13" s="122" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J13" s="114" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="K13">
+        <v>5</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D14" s="108">
         <v>14</v>
       </c>
       <c r="G14" s="122" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="H14">
+        <v>11</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J14" s="114" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D15" s="108">
         <v>15</v>
       </c>
       <c r="G15" s="122" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J15" s="114" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D16" s="108">
         <v>16</v>
       </c>
       <c r="G16" s="122" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="H16">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J16" s="114" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D17" s="108">
         <v>17</v>
       </c>
       <c r="G17" s="122" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="H17">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J17" s="114" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" s="108">
         <v>18</v>
       </c>
       <c r="G18" s="123" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="H18">
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J18" s="117" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D19" s="108">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D20" s="108">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D21" s="108">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D22" s="108">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D23" s="108">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D24" s="108">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D25" s="108">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D26" s="108">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D27" s="108">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D28" s="108">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D29" s="108">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D30" s="108">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D31" s="108">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D32" s="108">
         <v>32</v>
       </c>

</xml_diff>